<commit_message>
Run Read Data Changes
</commit_message>
<xml_diff>
--- a/fastexcel-reader/src/test/resources/xlsx/VeryHidden.xlsx
+++ b/fastexcel-reader/src/test/resources/xlsx/VeryHidden.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\broco\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1DBBC67C-3F43-4FE6-85B6-CA66D34A35FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{F3C9FE7C-CF8C-4393-8526-7CEAA3921AA3}"/>
+    <workbookView xWindow="0" yWindow="1125" windowWidth="11430" windowHeight="9375" firstSheet="2" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil1" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" state="veryHidden" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <oleSize ref="A1:K29"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +24,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -118,7 +116,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -170,7 +168,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -364,33 +362,69 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD05A622-19D3-48FA-B509-E01B41BFB644}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34B6827A-CC32-4B06-A3A3-9B2D5E3BCC89}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Feuil2"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>